<commit_message>
Renumber part and updated BOM
</commit_message>
<xml_diff>
--- a/EXM Relay Three/Rev A2/EXM Relay Three - Rev A2 - MDP/EXM Relay Three - Rev A2 - BOM.xlsx
+++ b/EXM Relay Three/Rev A2/EXM Relay Three - Rev A2 - MDP/EXM Relay Three - Rev A2 - BOM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adrian\Documents\ExMachina\repos\EXM\electronics\EXM Relay Three\Rev A1\EXM Relay Three - Rev A1 - MDP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adrian\Documents\ExMachina\repos\EXM\electronics\EXM Relay Three\Rev A2\EXM Relay Three - Rev A2 - MDP\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -53,15 +53,9 @@
     <t>Mount</t>
   </si>
   <si>
-    <t>J2, J3, J5, J6, J8, J9</t>
-  </si>
-  <si>
     <t>J10</t>
   </si>
   <si>
-    <t>J1, J4, J7</t>
-  </si>
-  <si>
     <t>K1, K2, K3</t>
   </si>
   <si>
@@ -77,9 +71,6 @@
     <t>OMRON COMPONENTS USA</t>
   </si>
   <si>
-    <t>22-05-7038</t>
-  </si>
-  <si>
     <t>1757242</t>
   </si>
   <si>
@@ -95,9 +86,6 @@
     <t>MOLEX</t>
   </si>
   <si>
-    <t>Connecteur fil-à-carte, Angle Droit, 2.54 mm, 3 Contact(s), Embase, Série KK </t>
-  </si>
-  <si>
     <t>Bornier, Embase, 5.08 mm, 2 Voies, 12 A, 250 V, Traversant angle droit</t>
   </si>
   <si>
@@ -114,6 +102,18 @@
   </si>
   <si>
     <t>Accessoire pour relais, MY/LY Series, Maintien bas</t>
+  </si>
+  <si>
+    <t>22-05-7048</t>
+  </si>
+  <si>
+    <t>Connecteur fil-à-carte, Angle Droit, 2.54 mm, 4 Contact(s), Embase, Série KK </t>
+  </si>
+  <si>
+    <t>J1, J2, J4, J5, J7, J8</t>
+  </si>
+  <si>
+    <t>J3, J6, J9</t>
   </si>
 </sst>
 </file>
@@ -523,7 +523,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,25 +570,25 @@
         <v>6</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>20</v>
-      </c>
       <c r="I2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -596,25 +596,25 @@
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="H3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="7" t="s">
         <v>18</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -622,25 +622,25 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -648,25 +648,25 @@
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -675,16 +675,16 @@
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>